<commit_message>
add chamfer & resolution_scale
</commit_message>
<xml_diff>
--- a/LYSO_test.xlsx
+++ b/LYSO_test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>LYSO:Ce</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>all black + black circle</t>
+  </si>
+  <si>
+    <t>all black + black circle + grease a lot</t>
+  </si>
+  <si>
+    <t>all black 2 + grease a lot</t>
+  </si>
+  <si>
+    <t>all black 2 + grease a lot + not center</t>
   </si>
 </sst>
 </file>
@@ -373,15 +382,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -413,14 +422,34 @@
       <c r="C4">
         <v>19979.099999999999</v>
       </c>
-      <c r="D4">
-        <f>(C3-C4)/C4</f>
-        <v>0.11746775380272392</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
+      </c>
+      <c r="C5">
+        <v>20614.900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>22001.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>22321.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>